<commit_message>
Update Table S1 with original references
</commit_message>
<xml_diff>
--- a/inputs/ChinookFullPanelLociTable_May2024Updated.xlsx
+++ b/inputs/ChinookFullPanelLociTable_May2024Updated.xlsx
@@ -1,23 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10414"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11028"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ellen/Genetics_Lab_Data/DataAnalysis/california-chinook-microhaps/inputs/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/eriq/Documents/git-repos/california-chinook-microhaps/inputs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{447DAB9B-8B6A-A647-A257-620F786333AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A042437D-39EF-864F-9CF1-52F9BA52A920}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5660" yWindow="880" windowWidth="27080" windowHeight="22400" xr2:uid="{E56130A1-82B1-034C-9FBF-E21DD198A6C4}"/>
+    <workbookView xWindow="5660" yWindow="760" windowWidth="27080" windowHeight="21580" xr2:uid="{E56130A1-82B1-034C-9FBF-E21DD198A6C4}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Key" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$U$205</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$V$205</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1885" uniqueCount="1474">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2089" uniqueCount="1479">
   <si>
     <t>ACTACAGGCACTCTCCCTGGCTAGAAGGGCAGGATAATAACAAACAAGAGATKATTTAAAGCCAGAGAAGTGATGGGGG</t>
   </si>
@@ -4461,13 +4461,28 @@
   </si>
   <si>
     <t>SNPtype</t>
+  </si>
+  <si>
+    <t>Original Reference</t>
+  </si>
+  <si>
+    <t>Clemento et al. 2014</t>
+  </si>
+  <si>
+    <t>Thompson et al. 2021</t>
+  </si>
+  <si>
+    <t>This study</t>
+  </si>
+  <si>
+    <t>Waters et al. 2021</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -4498,6 +4513,12 @@
       <b/>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -4926,10 +4947,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{575934F3-73D5-F049-89DB-6A73CBC8D927}">
-  <dimension ref="A1:U205"/>
+  <dimension ref="A1:V205"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K205" sqref="K205"/>
+    <sheetView tabSelected="1" topLeftCell="I159" workbookViewId="0">
+      <selection activeCell="L209" sqref="L209"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4943,10 +4964,11 @@
     <col min="9" max="9" width="61.5" customWidth="1"/>
     <col min="10" max="10" width="59.6640625" customWidth="1"/>
     <col min="11" max="11" width="12.1640625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="119.5" style="2" customWidth="1"/>
+    <col min="12" max="12" width="24.83203125" customWidth="1"/>
+    <col min="13" max="13" width="119.5" style="2" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="17" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:13" ht="17" x14ac:dyDescent="0.2">
       <c r="A1" s="5" t="s">
         <v>98</v>
       </c>
@@ -4980,11 +5002,14 @@
       <c r="K1" s="5" t="s">
         <v>1465</v>
       </c>
-      <c r="L1" s="6" t="s">
+      <c r="L1" s="5" t="s">
+        <v>1474</v>
+      </c>
+      <c r="M1" s="6" t="s">
         <v>303</v>
       </c>
     </row>
-    <row r="2" spans="1:12" s="13" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:13" s="13" customFormat="1" ht="17" x14ac:dyDescent="0.2">
       <c r="A2" s="13" t="s">
         <v>99</v>
       </c>
@@ -5015,11 +5040,14 @@
       <c r="K2" s="13" t="s">
         <v>1473</v>
       </c>
-      <c r="L2" s="14" t="s">
+      <c r="L2" s="13" t="s">
+        <v>1475</v>
+      </c>
+      <c r="M2" s="14" t="s">
         <v>1278</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>100</v>
       </c>
@@ -5047,8 +5075,11 @@
       <c r="K3" t="s">
         <v>1473</v>
       </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="L3" s="13" t="s">
+        <v>1475</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>101</v>
       </c>
@@ -5076,8 +5107,11 @@
       <c r="K4" t="s">
         <v>1473</v>
       </c>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="L4" s="13" t="s">
+        <v>1475</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>102</v>
       </c>
@@ -5105,8 +5139,11 @@
       <c r="K5" t="s">
         <v>1473</v>
       </c>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="L5" s="13" t="s">
+        <v>1475</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>103</v>
       </c>
@@ -5134,8 +5171,11 @@
       <c r="K6" t="s">
         <v>1473</v>
       </c>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="L6" s="13" t="s">
+        <v>1475</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>104</v>
       </c>
@@ -5163,8 +5203,11 @@
       <c r="K7" t="s">
         <v>1473</v>
       </c>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="L7" s="13" t="s">
+        <v>1475</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>105</v>
       </c>
@@ -5192,8 +5235,11 @@
       <c r="K8" t="s">
         <v>1473</v>
       </c>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="L8" s="13" t="s">
+        <v>1475</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>106</v>
       </c>
@@ -5221,8 +5267,11 @@
       <c r="K9" t="s">
         <v>1473</v>
       </c>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="L9" s="13" t="s">
+        <v>1475</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>107</v>
       </c>
@@ -5250,8 +5299,11 @@
       <c r="K10" t="s">
         <v>1473</v>
       </c>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="L10" s="13" t="s">
+        <v>1475</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>108</v>
       </c>
@@ -5279,8 +5331,11 @@
       <c r="K11" t="s">
         <v>1473</v>
       </c>
-    </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="L11" s="13" t="s">
+        <v>1475</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>109</v>
       </c>
@@ -5308,8 +5363,11 @@
       <c r="K12" t="s">
         <v>1473</v>
       </c>
-    </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="L12" s="13" t="s">
+        <v>1475</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>110</v>
       </c>
@@ -5337,8 +5395,11 @@
       <c r="K13" t="s">
         <v>1473</v>
       </c>
-    </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="L13" s="13" t="s">
+        <v>1475</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>111</v>
       </c>
@@ -5366,8 +5427,11 @@
       <c r="K14" t="s">
         <v>1473</v>
       </c>
-    </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="L14" s="13" t="s">
+        <v>1475</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>112</v>
       </c>
@@ -5395,8 +5459,11 @@
       <c r="K15" t="s">
         <v>1473</v>
       </c>
-    </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="L15" s="13" t="s">
+        <v>1475</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>113</v>
       </c>
@@ -5424,8 +5491,11 @@
       <c r="K16" t="s">
         <v>1473</v>
       </c>
-    </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="L16" s="13" t="s">
+        <v>1475</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>114</v>
       </c>
@@ -5453,8 +5523,11 @@
       <c r="K17" t="s">
         <v>1473</v>
       </c>
-    </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="L17" s="13" t="s">
+        <v>1475</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>115</v>
       </c>
@@ -5482,8 +5555,11 @@
       <c r="K18" t="s">
         <v>1473</v>
       </c>
-    </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="L18" s="13" t="s">
+        <v>1475</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>116</v>
       </c>
@@ -5511,8 +5587,11 @@
       <c r="K19" t="s">
         <v>1473</v>
       </c>
-    </row>
-    <row r="20" spans="1:12" s="13" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+      <c r="L19" s="13" t="s">
+        <v>1475</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13" s="13" customFormat="1" ht="17" x14ac:dyDescent="0.2">
       <c r="A20" s="13" t="s">
         <v>117</v>
       </c>
@@ -5543,11 +5622,14 @@
       <c r="K20" s="13" t="s">
         <v>1473</v>
       </c>
-      <c r="L20" s="14" t="s">
+      <c r="L20" s="13" t="s">
+        <v>1475</v>
+      </c>
+      <c r="M20" s="14" t="s">
         <v>1278</v>
       </c>
     </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>118</v>
       </c>
@@ -5575,8 +5657,11 @@
       <c r="K21" t="s">
         <v>1473</v>
       </c>
-    </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="L21" s="13" t="s">
+        <v>1475</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>119</v>
       </c>
@@ -5604,8 +5689,11 @@
       <c r="K22" t="s">
         <v>1473</v>
       </c>
-    </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="L22" s="13" t="s">
+        <v>1475</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>120</v>
       </c>
@@ -5633,8 +5721,11 @@
       <c r="K23" t="s">
         <v>1473</v>
       </c>
-    </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="L23" s="13" t="s">
+        <v>1475</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>121</v>
       </c>
@@ -5662,8 +5753,11 @@
       <c r="K24" t="s">
         <v>1473</v>
       </c>
-    </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="L24" s="13" t="s">
+        <v>1475</v>
+      </c>
+    </row>
+    <row r="25" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>122</v>
       </c>
@@ -5691,8 +5785,11 @@
       <c r="K25" t="s">
         <v>1473</v>
       </c>
-    </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="L25" s="13" t="s">
+        <v>1475</v>
+      </c>
+    </row>
+    <row r="26" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>123</v>
       </c>
@@ -5720,8 +5817,11 @@
       <c r="K26" t="s">
         <v>1473</v>
       </c>
-    </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="L26" s="13" t="s">
+        <v>1475</v>
+      </c>
+    </row>
+    <row r="27" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>124</v>
       </c>
@@ -5749,8 +5849,11 @@
       <c r="K27" t="s">
         <v>1473</v>
       </c>
-    </row>
-    <row r="28" spans="1:12" s="13" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+      <c r="L27" s="13" t="s">
+        <v>1475</v>
+      </c>
+    </row>
+    <row r="28" spans="1:13" s="13" customFormat="1" ht="17" x14ac:dyDescent="0.2">
       <c r="A28" s="13" t="s">
         <v>125</v>
       </c>
@@ -5781,11 +5884,14 @@
       <c r="K28" s="13" t="s">
         <v>1473</v>
       </c>
-      <c r="L28" s="14" t="s">
+      <c r="L28" s="13" t="s">
+        <v>1475</v>
+      </c>
+      <c r="M28" s="14" t="s">
         <v>1278</v>
       </c>
     </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>126</v>
       </c>
@@ -5813,8 +5919,11 @@
       <c r="K29" t="s">
         <v>1473</v>
       </c>
-    </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="L29" s="13" t="s">
+        <v>1475</v>
+      </c>
+    </row>
+    <row r="30" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>127</v>
       </c>
@@ -5842,8 +5951,11 @@
       <c r="K30" t="s">
         <v>1473</v>
       </c>
-    </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="L30" s="13" t="s">
+        <v>1475</v>
+      </c>
+    </row>
+    <row r="31" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>128</v>
       </c>
@@ -5871,8 +5983,11 @@
       <c r="K31" t="s">
         <v>1473</v>
       </c>
-    </row>
-    <row r="32" spans="1:12" s="13" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+      <c r="L31" s="13" t="s">
+        <v>1475</v>
+      </c>
+    </row>
+    <row r="32" spans="1:13" s="13" customFormat="1" ht="17" x14ac:dyDescent="0.2">
       <c r="A32" s="13" t="s">
         <v>129</v>
       </c>
@@ -5903,11 +6018,14 @@
       <c r="K32" s="13" t="s">
         <v>1473</v>
       </c>
-      <c r="L32" s="14" t="s">
+      <c r="L32" s="13" t="s">
+        <v>1475</v>
+      </c>
+      <c r="M32" s="14" t="s">
         <v>1278</v>
       </c>
     </row>
-    <row r="33" spans="1:12" s="13" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:13" s="13" customFormat="1" ht="17" x14ac:dyDescent="0.2">
       <c r="A33" s="13" t="s">
         <v>130</v>
       </c>
@@ -5938,11 +6056,14 @@
       <c r="K33" s="13" t="s">
         <v>1473</v>
       </c>
-      <c r="L33" s="14" t="s">
+      <c r="L33" s="13" t="s">
+        <v>1475</v>
+      </c>
+      <c r="M33" s="14" t="s">
         <v>1278</v>
       </c>
     </row>
-    <row r="34" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>131</v>
       </c>
@@ -5970,8 +6091,11 @@
       <c r="K34" t="s">
         <v>1473</v>
       </c>
-    </row>
-    <row r="35" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="L34" s="13" t="s">
+        <v>1475</v>
+      </c>
+    </row>
+    <row r="35" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>132</v>
       </c>
@@ -5999,8 +6123,11 @@
       <c r="K35" t="s">
         <v>1473</v>
       </c>
-    </row>
-    <row r="36" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="L35" s="13" t="s">
+        <v>1475</v>
+      </c>
+    </row>
+    <row r="36" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>133</v>
       </c>
@@ -6028,8 +6155,11 @@
       <c r="K36" t="s">
         <v>1473</v>
       </c>
-    </row>
-    <row r="37" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="L36" s="13" t="s">
+        <v>1475</v>
+      </c>
+    </row>
+    <row r="37" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>134</v>
       </c>
@@ -6057,8 +6187,11 @@
       <c r="K37" t="s">
         <v>1473</v>
       </c>
-    </row>
-    <row r="38" spans="1:12" s="13" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+      <c r="L37" s="13" t="s">
+        <v>1475</v>
+      </c>
+    </row>
+    <row r="38" spans="1:13" s="13" customFormat="1" ht="17" x14ac:dyDescent="0.2">
       <c r="A38" s="13" t="s">
         <v>135</v>
       </c>
@@ -6089,11 +6222,14 @@
       <c r="K38" s="13" t="s">
         <v>1473</v>
       </c>
-      <c r="L38" s="14" t="s">
+      <c r="L38" s="13" t="s">
+        <v>1475</v>
+      </c>
+      <c r="M38" s="14" t="s">
         <v>1278</v>
       </c>
     </row>
-    <row r="39" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>136</v>
       </c>
@@ -6121,8 +6257,11 @@
       <c r="K39" t="s">
         <v>1473</v>
       </c>
-    </row>
-    <row r="40" spans="1:12" s="9" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+      <c r="L39" s="13" t="s">
+        <v>1475</v>
+      </c>
+    </row>
+    <row r="40" spans="1:13" s="9" customFormat="1" ht="17" x14ac:dyDescent="0.2">
       <c r="A40" s="9" t="s">
         <v>137</v>
       </c>
@@ -6156,11 +6295,14 @@
       <c r="K40" s="9" t="s">
         <v>1473</v>
       </c>
-      <c r="L40" s="10" t="s">
+      <c r="L40" s="13" t="s">
+        <v>1475</v>
+      </c>
+      <c r="M40" s="10" t="s">
         <v>1291</v>
       </c>
     </row>
-    <row r="41" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>138</v>
       </c>
@@ -6188,8 +6330,11 @@
       <c r="K41" t="s">
         <v>1473</v>
       </c>
-    </row>
-    <row r="42" spans="1:12" s="20" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+      <c r="L41" s="13" t="s">
+        <v>1475</v>
+      </c>
+    </row>
+    <row r="42" spans="1:13" s="20" customFormat="1" ht="17" x14ac:dyDescent="0.2">
       <c r="A42" s="20" t="s">
         <v>139</v>
       </c>
@@ -6223,11 +6368,14 @@
       <c r="K42" s="20" t="s">
         <v>1473</v>
       </c>
-      <c r="L42" s="21" t="s">
+      <c r="L42" s="13" t="s">
+        <v>1475</v>
+      </c>
+      <c r="M42" s="21" t="s">
         <v>1277</v>
       </c>
     </row>
-    <row r="43" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>140</v>
       </c>
@@ -6255,8 +6403,11 @@
       <c r="K43" t="s">
         <v>1473</v>
       </c>
-    </row>
-    <row r="44" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="L43" s="13" t="s">
+        <v>1475</v>
+      </c>
+    </row>
+    <row r="44" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>141</v>
       </c>
@@ -6284,8 +6435,11 @@
       <c r="K44" t="s">
         <v>1473</v>
       </c>
-    </row>
-    <row r="45" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="L44" s="13" t="s">
+        <v>1475</v>
+      </c>
+    </row>
+    <row r="45" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>142</v>
       </c>
@@ -6313,8 +6467,11 @@
       <c r="K45" t="s">
         <v>1473</v>
       </c>
-    </row>
-    <row r="46" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="L45" s="13" t="s">
+        <v>1475</v>
+      </c>
+    </row>
+    <row r="46" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>143</v>
       </c>
@@ -6342,8 +6499,11 @@
       <c r="K46" t="s">
         <v>1473</v>
       </c>
-    </row>
-    <row r="47" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="L46" s="13" t="s">
+        <v>1475</v>
+      </c>
+    </row>
+    <row r="47" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>144</v>
       </c>
@@ -6371,8 +6531,11 @@
       <c r="K47" t="s">
         <v>1473</v>
       </c>
-    </row>
-    <row r="48" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="L47" s="13" t="s">
+        <v>1475</v>
+      </c>
+    </row>
+    <row r="48" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>145</v>
       </c>
@@ -6400,8 +6563,11 @@
       <c r="K48" t="s">
         <v>1473</v>
       </c>
-    </row>
-    <row r="49" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="L48" s="13" t="s">
+        <v>1475</v>
+      </c>
+    </row>
+    <row r="49" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>146</v>
       </c>
@@ -6429,8 +6595,11 @@
       <c r="K49" t="s">
         <v>1473</v>
       </c>
-    </row>
-    <row r="50" spans="1:12" s="13" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+      <c r="L49" s="13" t="s">
+        <v>1475</v>
+      </c>
+    </row>
+    <row r="50" spans="1:13" s="13" customFormat="1" ht="17" x14ac:dyDescent="0.2">
       <c r="A50" s="13" t="s">
         <v>147</v>
       </c>
@@ -6461,11 +6630,14 @@
       <c r="K50" s="13" t="s">
         <v>1473</v>
       </c>
-      <c r="L50" s="14" t="s">
+      <c r="L50" s="13" t="s">
+        <v>1475</v>
+      </c>
+      <c r="M50" s="14" t="s">
         <v>1278</v>
       </c>
     </row>
-    <row r="51" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>148</v>
       </c>
@@ -6493,8 +6665,11 @@
       <c r="K51" t="s">
         <v>1473</v>
       </c>
-    </row>
-    <row r="52" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="L51" s="13" t="s">
+        <v>1475</v>
+      </c>
+    </row>
+    <row r="52" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>149</v>
       </c>
@@ -6522,8 +6697,11 @@
       <c r="K52" t="s">
         <v>1473</v>
       </c>
-    </row>
-    <row r="53" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="L52" s="13" t="s">
+        <v>1475</v>
+      </c>
+    </row>
+    <row r="53" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>150</v>
       </c>
@@ -6551,8 +6729,11 @@
       <c r="K53" t="s">
         <v>1473</v>
       </c>
-    </row>
-    <row r="54" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="L53" s="13" t="s">
+        <v>1475</v>
+      </c>
+    </row>
+    <row r="54" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
         <v>151</v>
       </c>
@@ -6580,8 +6761,11 @@
       <c r="K54" t="s">
         <v>1473</v>
       </c>
-    </row>
-    <row r="55" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="L54" s="13" t="s">
+        <v>1475</v>
+      </c>
+    </row>
+    <row r="55" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
         <v>152</v>
       </c>
@@ -6609,8 +6793,11 @@
       <c r="K55" t="s">
         <v>1473</v>
       </c>
-    </row>
-    <row r="56" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="L55" s="13" t="s">
+        <v>1475</v>
+      </c>
+    </row>
+    <row r="56" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
         <v>153</v>
       </c>
@@ -6638,8 +6825,11 @@
       <c r="K56" t="s">
         <v>1473</v>
       </c>
-    </row>
-    <row r="57" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="L56" s="13" t="s">
+        <v>1475</v>
+      </c>
+    </row>
+    <row r="57" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
         <v>154</v>
       </c>
@@ -6667,8 +6857,11 @@
       <c r="K57" t="s">
         <v>1473</v>
       </c>
-    </row>
-    <row r="58" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="L57" s="13" t="s">
+        <v>1475</v>
+      </c>
+    </row>
+    <row r="58" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
         <v>155</v>
       </c>
@@ -6696,8 +6889,11 @@
       <c r="K58" t="s">
         <v>1473</v>
       </c>
-    </row>
-    <row r="59" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="L58" s="13" t="s">
+        <v>1475</v>
+      </c>
+    </row>
+    <row r="59" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
         <v>156</v>
       </c>
@@ -6725,8 +6921,11 @@
       <c r="K59" t="s">
         <v>1473</v>
       </c>
-    </row>
-    <row r="60" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="L59" s="13" t="s">
+        <v>1475</v>
+      </c>
+    </row>
+    <row r="60" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
         <v>157</v>
       </c>
@@ -6754,8 +6953,11 @@
       <c r="K60" t="s">
         <v>1473</v>
       </c>
-    </row>
-    <row r="61" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="L60" s="13" t="s">
+        <v>1475</v>
+      </c>
+    </row>
+    <row r="61" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
         <v>158</v>
       </c>
@@ -6783,8 +6985,11 @@
       <c r="K61" t="s">
         <v>1473</v>
       </c>
-    </row>
-    <row r="62" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="L61" s="13" t="s">
+        <v>1475</v>
+      </c>
+    </row>
+    <row r="62" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
         <v>159</v>
       </c>
@@ -6812,8 +7017,11 @@
       <c r="K62" t="s">
         <v>1473</v>
       </c>
-    </row>
-    <row r="63" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="L62" s="13" t="s">
+        <v>1475</v>
+      </c>
+    </row>
+    <row r="63" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
         <v>160</v>
       </c>
@@ -6841,8 +7049,11 @@
       <c r="K63" t="s">
         <v>1473</v>
       </c>
-    </row>
-    <row r="64" spans="1:12" s="11" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+      <c r="L63" s="13" t="s">
+        <v>1475</v>
+      </c>
+    </row>
+    <row r="64" spans="1:13" s="11" customFormat="1" ht="17" x14ac:dyDescent="0.2">
       <c r="A64" s="11" t="s">
         <v>161</v>
       </c>
@@ -6873,11 +7084,14 @@
       <c r="K64" s="11" t="s">
         <v>1473</v>
       </c>
-      <c r="L64" s="12" t="s">
+      <c r="L64" s="13" t="s">
+        <v>1475</v>
+      </c>
+      <c r="M64" s="12" t="s">
         <v>1280</v>
       </c>
     </row>
-    <row r="65" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
         <v>162</v>
       </c>
@@ -6905,8 +7119,11 @@
       <c r="K65" t="s">
         <v>1473</v>
       </c>
-    </row>
-    <row r="66" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="L65" s="13" t="s">
+        <v>1475</v>
+      </c>
+    </row>
+    <row r="66" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
         <v>163</v>
       </c>
@@ -6934,8 +7151,11 @@
       <c r="K66" t="s">
         <v>1473</v>
       </c>
-    </row>
-    <row r="67" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="L66" s="13" t="s">
+        <v>1475</v>
+      </c>
+    </row>
+    <row r="67" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
         <v>164</v>
       </c>
@@ -6963,8 +7183,11 @@
       <c r="K67" t="s">
         <v>1473</v>
       </c>
-    </row>
-    <row r="68" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="L67" s="13" t="s">
+        <v>1475</v>
+      </c>
+    </row>
+    <row r="68" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
         <v>165</v>
       </c>
@@ -6992,8 +7215,11 @@
       <c r="K68" t="s">
         <v>1473</v>
       </c>
-    </row>
-    <row r="69" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="L68" s="13" t="s">
+        <v>1475</v>
+      </c>
+    </row>
+    <row r="69" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
         <v>166</v>
       </c>
@@ -7021,8 +7247,11 @@
       <c r="K69" t="s">
         <v>1473</v>
       </c>
-    </row>
-    <row r="70" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="L69" s="13" t="s">
+        <v>1475</v>
+      </c>
+    </row>
+    <row r="70" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
         <v>167</v>
       </c>
@@ -7050,8 +7279,11 @@
       <c r="K70" t="s">
         <v>1473</v>
       </c>
-    </row>
-    <row r="71" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="L70" s="13" t="s">
+        <v>1475</v>
+      </c>
+    </row>
+    <row r="71" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
         <v>168</v>
       </c>
@@ -7079,8 +7311,11 @@
       <c r="K71" t="s">
         <v>1473</v>
       </c>
-    </row>
-    <row r="72" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="L71" s="13" t="s">
+        <v>1475</v>
+      </c>
+    </row>
+    <row r="72" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
         <v>169</v>
       </c>
@@ -7108,8 +7343,11 @@
       <c r="K72" t="s">
         <v>1473</v>
       </c>
-    </row>
-    <row r="73" spans="1:12" s="13" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+      <c r="L72" s="13" t="s">
+        <v>1475</v>
+      </c>
+    </row>
+    <row r="73" spans="1:13" s="13" customFormat="1" ht="17" x14ac:dyDescent="0.2">
       <c r="A73" s="13" t="s">
         <v>170</v>
       </c>
@@ -7140,11 +7378,14 @@
       <c r="K73" s="13" t="s">
         <v>1473</v>
       </c>
-      <c r="L73" s="14" t="s">
+      <c r="L73" s="13" t="s">
+        <v>1475</v>
+      </c>
+      <c r="M73" s="14" t="s">
         <v>1278</v>
       </c>
     </row>
-    <row r="74" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
         <v>171</v>
       </c>
@@ -7172,8 +7413,11 @@
       <c r="K74" t="s">
         <v>1473</v>
       </c>
-    </row>
-    <row r="75" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="L74" s="13" t="s">
+        <v>1475</v>
+      </c>
+    </row>
+    <row r="75" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
         <v>172</v>
       </c>
@@ -7201,8 +7445,11 @@
       <c r="K75" t="s">
         <v>1473</v>
       </c>
-    </row>
-    <row r="76" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="L75" s="13" t="s">
+        <v>1475</v>
+      </c>
+    </row>
+    <row r="76" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
         <v>173</v>
       </c>
@@ -7230,8 +7477,11 @@
       <c r="K76" t="s">
         <v>1473</v>
       </c>
-    </row>
-    <row r="77" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="L76" s="13" t="s">
+        <v>1475</v>
+      </c>
+    </row>
+    <row r="77" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
         <v>174</v>
       </c>
@@ -7259,8 +7509,11 @@
       <c r="K77" t="s">
         <v>1473</v>
       </c>
-    </row>
-    <row r="78" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="L77" s="13" t="s">
+        <v>1475</v>
+      </c>
+    </row>
+    <row r="78" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
         <v>175</v>
       </c>
@@ -7288,8 +7541,11 @@
       <c r="K78" t="s">
         <v>1473</v>
       </c>
-    </row>
-    <row r="79" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="L78" s="13" t="s">
+        <v>1475</v>
+      </c>
+    </row>
+    <row r="79" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
         <v>176</v>
       </c>
@@ -7317,8 +7573,11 @@
       <c r="K79" t="s">
         <v>1473</v>
       </c>
-    </row>
-    <row r="80" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="L79" s="13" t="s">
+        <v>1475</v>
+      </c>
+    </row>
+    <row r="80" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
         <v>177</v>
       </c>
@@ -7346,8 +7605,11 @@
       <c r="K80" t="s">
         <v>1473</v>
       </c>
-    </row>
-    <row r="81" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="L80" s="13" t="s">
+        <v>1475</v>
+      </c>
+    </row>
+    <row r="81" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
         <v>178</v>
       </c>
@@ -7375,8 +7637,11 @@
       <c r="K81" t="s">
         <v>1472</v>
       </c>
-    </row>
-    <row r="82" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="L81" s="13" t="s">
+        <v>1476</v>
+      </c>
+    </row>
+    <row r="82" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
         <v>179</v>
       </c>
@@ -7404,8 +7669,11 @@
       <c r="K82" t="s">
         <v>1472</v>
       </c>
-    </row>
-    <row r="83" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="L82" s="13" t="s">
+        <v>1476</v>
+      </c>
+    </row>
+    <row r="83" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
         <v>180</v>
       </c>
@@ -7433,8 +7701,11 @@
       <c r="K83" t="s">
         <v>1472</v>
       </c>
-    </row>
-    <row r="84" spans="1:21" s="7" customFormat="1" ht="51" x14ac:dyDescent="0.2">
+      <c r="L83" s="13" t="s">
+        <v>1476</v>
+      </c>
+    </row>
+    <row r="84" spans="1:22" s="7" customFormat="1" ht="51" x14ac:dyDescent="0.2">
       <c r="A84" s="7" t="s">
         <v>181</v>
       </c>
@@ -7462,11 +7733,14 @@
       <c r="K84" s="7" t="s">
         <v>1472</v>
       </c>
-      <c r="L84" s="8" t="s">
+      <c r="L84" s="13" t="s">
+        <v>1476</v>
+      </c>
+      <c r="M84" s="8" t="s">
         <v>1275</v>
       </c>
     </row>
-    <row r="85" spans="1:21" s="11" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:22" s="11" customFormat="1" ht="17" x14ac:dyDescent="0.2">
       <c r="A85" s="11" t="s">
         <v>182</v>
       </c>
@@ -7497,11 +7771,14 @@
       <c r="K85" s="11" t="s">
         <v>1472</v>
       </c>
-      <c r="L85" s="12" t="s">
+      <c r="L85" s="13" t="s">
+        <v>1476</v>
+      </c>
+      <c r="M85" s="12" t="s">
         <v>1280</v>
       </c>
     </row>
-    <row r="86" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
         <v>183</v>
       </c>
@@ -7529,8 +7806,11 @@
       <c r="K86" t="s">
         <v>1472</v>
       </c>
-    </row>
-    <row r="87" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="L86" s="13" t="s">
+        <v>1476</v>
+      </c>
+    </row>
+    <row r="87" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
         <v>184</v>
       </c>
@@ -7558,8 +7838,11 @@
       <c r="K87" t="s">
         <v>1472</v>
       </c>
-    </row>
-    <row r="88" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="L87" s="13" t="s">
+        <v>1476</v>
+      </c>
+    </row>
+    <row r="88" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
         <v>185</v>
       </c>
@@ -7587,8 +7870,11 @@
       <c r="K88" t="s">
         <v>1472</v>
       </c>
-    </row>
-    <row r="89" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="L88" s="13" t="s">
+        <v>1476</v>
+      </c>
+    </row>
+    <row r="89" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
         <v>186</v>
       </c>
@@ -7616,8 +7902,11 @@
       <c r="K89" t="s">
         <v>1472</v>
       </c>
-    </row>
-    <row r="90" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="L89" s="13" t="s">
+        <v>1476</v>
+      </c>
+    </row>
+    <row r="90" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
         <v>187</v>
       </c>
@@ -7645,9 +7934,12 @@
       <c r="K90" t="s">
         <v>1472</v>
       </c>
-      <c r="O90" s="1"/>
-    </row>
-    <row r="91" spans="1:21" s="13" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+      <c r="L90" s="13" t="s">
+        <v>1476</v>
+      </c>
+      <c r="P90" s="1"/>
+    </row>
+    <row r="91" spans="1:22" s="13" customFormat="1" ht="17" x14ac:dyDescent="0.2">
       <c r="A91" s="13" t="s">
         <v>188</v>
       </c>
@@ -7678,18 +7970,21 @@
       <c r="K91" s="13" t="s">
         <v>1472</v>
       </c>
-      <c r="L91" s="14" t="s">
+      <c r="L91" s="13" t="s">
+        <v>1476</v>
+      </c>
+      <c r="M91" s="14" t="s">
         <v>1278</v>
       </c>
-      <c r="O91" s="15"/>
       <c r="P91" s="15"/>
       <c r="Q91" s="15"/>
       <c r="R91" s="15"/>
       <c r="S91" s="15"/>
       <c r="T91" s="15"/>
       <c r="U91" s="15"/>
-    </row>
-    <row r="92" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="V91" s="15"/>
+    </row>
+    <row r="92" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
         <v>189</v>
       </c>
@@ -7717,8 +8012,11 @@
       <c r="K92" t="s">
         <v>1472</v>
       </c>
-    </row>
-    <row r="93" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="L92" s="13" t="s">
+        <v>1476</v>
+      </c>
+    </row>
+    <row r="93" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
         <v>190</v>
       </c>
@@ -7746,8 +8044,11 @@
       <c r="K93" t="s">
         <v>1472</v>
       </c>
-    </row>
-    <row r="94" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="L93" s="13" t="s">
+        <v>1476</v>
+      </c>
+    </row>
+    <row r="94" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
         <v>191</v>
       </c>
@@ -7775,8 +8076,11 @@
       <c r="K94" t="s">
         <v>1472</v>
       </c>
-    </row>
-    <row r="95" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="L94" s="13" t="s">
+        <v>1476</v>
+      </c>
+    </row>
+    <row r="95" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
         <v>192</v>
       </c>
@@ -7804,8 +8108,11 @@
       <c r="K95" t="s">
         <v>1472</v>
       </c>
-    </row>
-    <row r="96" spans="1:21" s="16" customFormat="1" ht="102" x14ac:dyDescent="0.2">
+      <c r="L95" s="13" t="s">
+        <v>1476</v>
+      </c>
+    </row>
+    <row r="96" spans="1:22" s="16" customFormat="1" ht="102" x14ac:dyDescent="0.2">
       <c r="A96" s="16" t="s">
         <v>193</v>
       </c>
@@ -7839,11 +8146,14 @@
       <c r="K96" s="16" t="s">
         <v>1472</v>
       </c>
-      <c r="L96" s="17" t="s">
+      <c r="L96" s="13" t="s">
+        <v>1476</v>
+      </c>
+      <c r="M96" s="17" t="s">
         <v>1290</v>
       </c>
     </row>
-    <row r="97" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
         <v>194</v>
       </c>
@@ -7871,8 +8181,11 @@
       <c r="K97" t="s">
         <v>1472</v>
       </c>
-    </row>
-    <row r="98" spans="1:12" s="13" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+      <c r="L97" s="13" t="s">
+        <v>1476</v>
+      </c>
+    </row>
+    <row r="98" spans="1:13" s="13" customFormat="1" ht="17" x14ac:dyDescent="0.2">
       <c r="A98" s="13" t="s">
         <v>195</v>
       </c>
@@ -7903,11 +8216,14 @@
       <c r="K98" s="13" t="s">
         <v>1472</v>
       </c>
-      <c r="L98" s="14" t="s">
+      <c r="L98" s="13" t="s">
+        <v>1476</v>
+      </c>
+      <c r="M98" s="14" t="s">
         <v>1278</v>
       </c>
     </row>
-    <row r="99" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
         <v>196</v>
       </c>
@@ -7935,8 +8251,11 @@
       <c r="K99" t="s">
         <v>1472</v>
       </c>
-    </row>
-    <row r="100" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="L99" s="13" t="s">
+        <v>1476</v>
+      </c>
+    </row>
+    <row r="100" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
         <v>197</v>
       </c>
@@ -7964,8 +8283,11 @@
       <c r="K100" t="s">
         <v>1472</v>
       </c>
-    </row>
-    <row r="101" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="L100" s="13" t="s">
+        <v>1476</v>
+      </c>
+    </row>
+    <row r="101" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
         <v>198</v>
       </c>
@@ -7993,8 +8315,11 @@
       <c r="K101" t="s">
         <v>1472</v>
       </c>
-    </row>
-    <row r="102" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="L101" s="13" t="s">
+        <v>1476</v>
+      </c>
+    </row>
+    <row r="102" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
         <v>199</v>
       </c>
@@ -8022,8 +8347,11 @@
       <c r="K102" t="s">
         <v>1472</v>
       </c>
-    </row>
-    <row r="103" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="L102" s="13" t="s">
+        <v>1476</v>
+      </c>
+    </row>
+    <row r="103" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
         <v>200</v>
       </c>
@@ -8051,8 +8379,11 @@
       <c r="K103" t="s">
         <v>1472</v>
       </c>
-    </row>
-    <row r="104" spans="1:12" s="13" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+      <c r="L103" s="13" t="s">
+        <v>1476</v>
+      </c>
+    </row>
+    <row r="104" spans="1:13" s="13" customFormat="1" ht="17" x14ac:dyDescent="0.2">
       <c r="A104" s="13" t="s">
         <v>201</v>
       </c>
@@ -8083,11 +8414,14 @@
       <c r="K104" s="13" t="s">
         <v>1472</v>
       </c>
-      <c r="L104" s="14" t="s">
+      <c r="L104" s="13" t="s">
+        <v>1476</v>
+      </c>
+      <c r="M104" s="14" t="s">
         <v>1278</v>
       </c>
     </row>
-    <row r="105" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
         <v>202</v>
       </c>
@@ -8115,8 +8449,11 @@
       <c r="K105" t="s">
         <v>1472</v>
       </c>
-    </row>
-    <row r="106" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="L105" s="13" t="s">
+        <v>1476</v>
+      </c>
+    </row>
+    <row r="106" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
         <v>203</v>
       </c>
@@ -8144,8 +8481,11 @@
       <c r="K106" t="s">
         <v>1472</v>
       </c>
-    </row>
-    <row r="107" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="L106" s="13" t="s">
+        <v>1476</v>
+      </c>
+    </row>
+    <row r="107" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
         <v>204</v>
       </c>
@@ -8173,8 +8513,11 @@
       <c r="K107" t="s">
         <v>1472</v>
       </c>
-    </row>
-    <row r="108" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="L107" s="13" t="s">
+        <v>1476</v>
+      </c>
+    </row>
+    <row r="108" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A108" t="s">
         <v>205</v>
       </c>
@@ -8202,8 +8545,11 @@
       <c r="K108" t="s">
         <v>1472</v>
       </c>
-    </row>
-    <row r="109" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="L108" s="13" t="s">
+        <v>1476</v>
+      </c>
+    </row>
+    <row r="109" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A109" t="s">
         <v>206</v>
       </c>
@@ -8231,8 +8577,11 @@
       <c r="K109" t="s">
         <v>1472</v>
       </c>
-    </row>
-    <row r="110" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="L109" s="13" t="s">
+        <v>1476</v>
+      </c>
+    </row>
+    <row r="110" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A110" t="s">
         <v>207</v>
       </c>
@@ -8260,8 +8609,11 @@
       <c r="K110" t="s">
         <v>1472</v>
       </c>
-    </row>
-    <row r="111" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="L110" s="13" t="s">
+        <v>1476</v>
+      </c>
+    </row>
+    <row r="111" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A111" t="s">
         <v>208</v>
       </c>
@@ -8289,8 +8641,11 @@
       <c r="K111" t="s">
         <v>1472</v>
       </c>
-    </row>
-    <row r="112" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="L111" s="13" t="s">
+        <v>1476</v>
+      </c>
+    </row>
+    <row r="112" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A112" t="s">
         <v>209</v>
       </c>
@@ -8318,8 +8673,11 @@
       <c r="K112" t="s">
         <v>1472</v>
       </c>
-    </row>
-    <row r="113" spans="1:12" s="13" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+      <c r="L112" s="13" t="s">
+        <v>1476</v>
+      </c>
+    </row>
+    <row r="113" spans="1:13" s="13" customFormat="1" ht="17" x14ac:dyDescent="0.2">
       <c r="A113" s="13" t="s">
         <v>210</v>
       </c>
@@ -8350,11 +8708,14 @@
       <c r="K113" s="13" t="s">
         <v>1472</v>
       </c>
-      <c r="L113" s="14" t="s">
+      <c r="L113" s="13" t="s">
+        <v>1476</v>
+      </c>
+      <c r="M113" s="14" t="s">
         <v>1278</v>
       </c>
     </row>
-    <row r="114" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="114" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A114" t="s">
         <v>211</v>
       </c>
@@ -8382,8 +8743,11 @@
       <c r="K114" t="s">
         <v>1472</v>
       </c>
-    </row>
-    <row r="115" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="L114" s="13" t="s">
+        <v>1476</v>
+      </c>
+    </row>
+    <row r="115" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A115" t="s">
         <v>212</v>
       </c>
@@ -8411,8 +8775,11 @@
       <c r="K115" t="s">
         <v>1472</v>
       </c>
-    </row>
-    <row r="116" spans="1:12" s="13" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+      <c r="L115" s="13" t="s">
+        <v>1476</v>
+      </c>
+    </row>
+    <row r="116" spans="1:13" s="13" customFormat="1" ht="17" x14ac:dyDescent="0.2">
       <c r="A116" s="13" t="s">
         <v>213</v>
       </c>
@@ -8443,11 +8810,14 @@
       <c r="K116" s="13" t="s">
         <v>1472</v>
       </c>
-      <c r="L116" s="14" t="s">
+      <c r="L116" s="13" t="s">
+        <v>1476</v>
+      </c>
+      <c r="M116" s="14" t="s">
         <v>1278</v>
       </c>
     </row>
-    <row r="117" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="117" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A117" t="s">
         <v>214</v>
       </c>
@@ -8475,8 +8845,11 @@
       <c r="K117" t="s">
         <v>1472</v>
       </c>
-    </row>
-    <row r="118" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="L117" s="13" t="s">
+        <v>1476</v>
+      </c>
+    </row>
+    <row r="118" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A118" t="s">
         <v>215</v>
       </c>
@@ -8504,8 +8877,11 @@
       <c r="K118" t="s">
         <v>1472</v>
       </c>
-    </row>
-    <row r="119" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="L118" s="13" t="s">
+        <v>1476</v>
+      </c>
+    </row>
+    <row r="119" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A119" t="s">
         <v>216</v>
       </c>
@@ -8533,8 +8909,11 @@
       <c r="K119" t="s">
         <v>1472</v>
       </c>
-    </row>
-    <row r="120" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="L119" s="13" t="s">
+        <v>1476</v>
+      </c>
+    </row>
+    <row r="120" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A120" t="s">
         <v>217</v>
       </c>
@@ -8562,8 +8941,11 @@
       <c r="K120" t="s">
         <v>1472</v>
       </c>
-    </row>
-    <row r="121" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="L120" s="13" t="s">
+        <v>1476</v>
+      </c>
+    </row>
+    <row r="121" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A121" t="s">
         <v>218</v>
       </c>
@@ -8591,8 +8973,11 @@
       <c r="K121" t="s">
         <v>1472</v>
       </c>
-    </row>
-    <row r="122" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="L121" s="13" t="s">
+        <v>1476</v>
+      </c>
+    </row>
+    <row r="122" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A122" t="s">
         <v>219</v>
       </c>
@@ -8620,8 +9005,11 @@
       <c r="K122" t="s">
         <v>1472</v>
       </c>
-    </row>
-    <row r="123" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="L122" s="13" t="s">
+        <v>1476</v>
+      </c>
+    </row>
+    <row r="123" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A123" t="s">
         <v>220</v>
       </c>
@@ -8649,8 +9037,11 @@
       <c r="K123" t="s">
         <v>1472</v>
       </c>
-    </row>
-    <row r="124" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="L123" s="13" t="s">
+        <v>1476</v>
+      </c>
+    </row>
+    <row r="124" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A124" t="s">
         <v>221</v>
       </c>
@@ -8678,8 +9069,11 @@
       <c r="K124" t="s">
         <v>1472</v>
       </c>
-    </row>
-    <row r="125" spans="1:12" s="13" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+      <c r="L124" s="13" t="s">
+        <v>1476</v>
+      </c>
+    </row>
+    <row r="125" spans="1:13" s="13" customFormat="1" ht="17" x14ac:dyDescent="0.2">
       <c r="A125" s="13" t="s">
         <v>222</v>
       </c>
@@ -8710,11 +9104,14 @@
       <c r="K125" s="13" t="s">
         <v>1472</v>
       </c>
-      <c r="L125" s="14" t="s">
+      <c r="L125" s="13" t="s">
+        <v>1476</v>
+      </c>
+      <c r="M125" s="14" t="s">
         <v>1278</v>
       </c>
     </row>
-    <row r="126" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="126" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A126" t="s">
         <v>223</v>
       </c>
@@ -8742,8 +9139,11 @@
       <c r="K126" t="s">
         <v>1472</v>
       </c>
-    </row>
-    <row r="127" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="L126" s="13" t="s">
+        <v>1476</v>
+      </c>
+    </row>
+    <row r="127" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A127" t="s">
         <v>224</v>
       </c>
@@ -8771,8 +9171,11 @@
       <c r="K127" t="s">
         <v>1472</v>
       </c>
-    </row>
-    <row r="128" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="L127" s="13" t="s">
+        <v>1476</v>
+      </c>
+    </row>
+    <row r="128" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A128" t="s">
         <v>225</v>
       </c>
@@ -8800,8 +9203,11 @@
       <c r="K128" t="s">
         <v>1472</v>
       </c>
-    </row>
-    <row r="129" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="L128" s="13" t="s">
+        <v>1476</v>
+      </c>
+    </row>
+    <row r="129" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A129" t="s">
         <v>226</v>
       </c>
@@ -8829,8 +9235,11 @@
       <c r="K129" t="s">
         <v>1472</v>
       </c>
-    </row>
-    <row r="130" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="L129" s="13" t="s">
+        <v>1476</v>
+      </c>
+    </row>
+    <row r="130" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A130" t="s">
         <v>227</v>
       </c>
@@ -8858,8 +9267,11 @@
       <c r="K130" t="s">
         <v>1472</v>
       </c>
-    </row>
-    <row r="131" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="L130" s="13" t="s">
+        <v>1476</v>
+      </c>
+    </row>
+    <row r="131" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A131" t="s">
         <v>228</v>
       </c>
@@ -8887,8 +9299,11 @@
       <c r="K131" t="s">
         <v>1472</v>
       </c>
-    </row>
-    <row r="132" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="L131" s="13" t="s">
+        <v>1476</v>
+      </c>
+    </row>
+    <row r="132" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A132" t="s">
         <v>229</v>
       </c>
@@ -8916,8 +9331,11 @@
       <c r="K132" t="s">
         <v>1472</v>
       </c>
-    </row>
-    <row r="133" spans="1:12" s="13" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+      <c r="L132" s="13" t="s">
+        <v>1476</v>
+      </c>
+    </row>
+    <row r="133" spans="1:13" s="13" customFormat="1" ht="17" x14ac:dyDescent="0.2">
       <c r="A133" s="13" t="s">
         <v>230</v>
       </c>
@@ -8948,11 +9366,14 @@
       <c r="K133" s="13" t="s">
         <v>1472</v>
       </c>
-      <c r="L133" s="14" t="s">
+      <c r="L133" s="13" t="s">
+        <v>1476</v>
+      </c>
+      <c r="M133" s="14" t="s">
         <v>1278</v>
       </c>
     </row>
-    <row r="134" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="134" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A134" t="s">
         <v>231</v>
       </c>
@@ -8980,8 +9401,11 @@
       <c r="K134" t="s">
         <v>1472</v>
       </c>
-    </row>
-    <row r="135" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="L134" s="13" t="s">
+        <v>1476</v>
+      </c>
+    </row>
+    <row r="135" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A135" t="s">
         <v>232</v>
       </c>
@@ -9009,8 +9433,11 @@
       <c r="K135" t="s">
         <v>1472</v>
       </c>
-    </row>
-    <row r="136" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="L135" s="13" t="s">
+        <v>1476</v>
+      </c>
+    </row>
+    <row r="136" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A136" t="s">
         <v>233</v>
       </c>
@@ -9038,8 +9465,11 @@
       <c r="K136" t="s">
         <v>1472</v>
       </c>
-    </row>
-    <row r="137" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="L136" s="13" t="s">
+        <v>1476</v>
+      </c>
+    </row>
+    <row r="137" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A137" t="s">
         <v>234</v>
       </c>
@@ -9067,8 +9497,11 @@
       <c r="K137" t="s">
         <v>1472</v>
       </c>
-    </row>
-    <row r="138" spans="1:12" s="13" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+      <c r="L137" s="13" t="s">
+        <v>1476</v>
+      </c>
+    </row>
+    <row r="138" spans="1:13" s="13" customFormat="1" ht="17" x14ac:dyDescent="0.2">
       <c r="A138" s="13" t="s">
         <v>235</v>
       </c>
@@ -9099,11 +9532,14 @@
       <c r="K138" s="13" t="s">
         <v>1472</v>
       </c>
-      <c r="L138" s="14" t="s">
+      <c r="L138" s="13" t="s">
+        <v>1476</v>
+      </c>
+      <c r="M138" s="14" t="s">
         <v>1278</v>
       </c>
     </row>
-    <row r="139" spans="1:12" s="13" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+    <row r="139" spans="1:13" s="13" customFormat="1" ht="17" x14ac:dyDescent="0.2">
       <c r="A139" s="13" t="s">
         <v>236</v>
       </c>
@@ -9134,11 +9570,14 @@
       <c r="K139" s="13" t="s">
         <v>1472</v>
       </c>
-      <c r="L139" s="14" t="s">
+      <c r="L139" s="13" t="s">
+        <v>1476</v>
+      </c>
+      <c r="M139" s="14" t="s">
         <v>1278</v>
       </c>
     </row>
-    <row r="140" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="140" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A140" t="s">
         <v>237</v>
       </c>
@@ -9166,8 +9605,11 @@
       <c r="K140" t="s">
         <v>1472</v>
       </c>
-    </row>
-    <row r="141" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="L140" s="13" t="s">
+        <v>1476</v>
+      </c>
+    </row>
+    <row r="141" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A141" t="s">
         <v>238</v>
       </c>
@@ -9195,8 +9637,11 @@
       <c r="K141" t="s">
         <v>1472</v>
       </c>
-    </row>
-    <row r="142" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="L141" s="13" t="s">
+        <v>1476</v>
+      </c>
+    </row>
+    <row r="142" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A142" t="s">
         <v>239</v>
       </c>
@@ -9224,8 +9669,11 @@
       <c r="K142" t="s">
         <v>1472</v>
       </c>
-    </row>
-    <row r="143" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="L142" s="13" t="s">
+        <v>1476</v>
+      </c>
+    </row>
+    <row r="143" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A143" t="s">
         <v>240</v>
       </c>
@@ -9253,8 +9701,11 @@
       <c r="K143" t="s">
         <v>1472</v>
       </c>
-    </row>
-    <row r="144" spans="1:12" s="13" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+      <c r="L143" s="13" t="s">
+        <v>1476</v>
+      </c>
+    </row>
+    <row r="144" spans="1:13" s="13" customFormat="1" ht="17" x14ac:dyDescent="0.2">
       <c r="A144" s="13" t="s">
         <v>241</v>
       </c>
@@ -9285,11 +9736,14 @@
       <c r="K144" s="13" t="s">
         <v>1472</v>
       </c>
-      <c r="L144" s="14" t="s">
+      <c r="L144" s="13" t="s">
+        <v>1476</v>
+      </c>
+      <c r="M144" s="14" t="s">
         <v>1278</v>
       </c>
     </row>
-    <row r="145" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="145" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A145" t="s">
         <v>242</v>
       </c>
@@ -9317,8 +9771,11 @@
       <c r="K145" t="s">
         <v>1472</v>
       </c>
-    </row>
-    <row r="146" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="L145" s="13" t="s">
+        <v>1476</v>
+      </c>
+    </row>
+    <row r="146" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A146" t="s">
         <v>243</v>
       </c>
@@ -9346,8 +9803,11 @@
       <c r="K146" t="s">
         <v>1472</v>
       </c>
-    </row>
-    <row r="147" spans="1:12" s="13" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+      <c r="L146" s="13" t="s">
+        <v>1476</v>
+      </c>
+    </row>
+    <row r="147" spans="1:13" s="13" customFormat="1" ht="17" x14ac:dyDescent="0.2">
       <c r="A147" s="13" t="s">
         <v>244</v>
       </c>
@@ -9378,11 +9838,14 @@
       <c r="K147" s="13" t="s">
         <v>1472</v>
       </c>
-      <c r="L147" s="14" t="s">
+      <c r="L147" s="13" t="s">
+        <v>1476</v>
+      </c>
+      <c r="M147" s="14" t="s">
         <v>1278</v>
       </c>
     </row>
-    <row r="148" spans="1:12" s="18" customFormat="1" ht="34" x14ac:dyDescent="0.2">
+    <row r="148" spans="1:13" s="18" customFormat="1" ht="34" x14ac:dyDescent="0.2">
       <c r="A148" s="18" t="s">
         <v>245</v>
       </c>
@@ -9410,11 +9873,14 @@
       <c r="K148" s="18" t="s">
         <v>1472</v>
       </c>
-      <c r="L148" s="19" t="s">
+      <c r="L148" s="13" t="s">
+        <v>1476</v>
+      </c>
+      <c r="M148" s="19" t="s">
         <v>1287</v>
       </c>
     </row>
-    <row r="149" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="149" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A149" t="s">
         <v>246</v>
       </c>
@@ -9442,8 +9908,11 @@
       <c r="K149" t="s">
         <v>1472</v>
       </c>
-    </row>
-    <row r="150" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="L149" s="13" t="s">
+        <v>1476</v>
+      </c>
+    </row>
+    <row r="150" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A150" t="s">
         <v>247</v>
       </c>
@@ -9471,8 +9940,11 @@
       <c r="K150" t="s">
         <v>1472</v>
       </c>
-    </row>
-    <row r="151" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="L150" s="13" t="s">
+        <v>1476</v>
+      </c>
+    </row>
+    <row r="151" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A151" t="s">
         <v>248</v>
       </c>
@@ -9500,8 +9972,11 @@
       <c r="K151" t="s">
         <v>1472</v>
       </c>
-    </row>
-    <row r="152" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="L151" s="13" t="s">
+        <v>1476</v>
+      </c>
+    </row>
+    <row r="152" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A152" t="s">
         <v>249</v>
       </c>
@@ -9529,8 +10004,11 @@
       <c r="K152" t="s">
         <v>1472</v>
       </c>
-    </row>
-    <row r="153" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="L152" s="13" t="s">
+        <v>1476</v>
+      </c>
+    </row>
+    <row r="153" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A153" t="s">
         <v>250</v>
       </c>
@@ -9558,8 +10036,11 @@
       <c r="K153" t="s">
         <v>1472</v>
       </c>
-    </row>
-    <row r="154" spans="1:12" s="7" customFormat="1" ht="34" x14ac:dyDescent="0.2">
+      <c r="L153" s="13" t="s">
+        <v>1476</v>
+      </c>
+    </row>
+    <row r="154" spans="1:13" s="7" customFormat="1" ht="34" x14ac:dyDescent="0.2">
       <c r="A154" s="7" t="s">
         <v>251</v>
       </c>
@@ -9587,11 +10068,14 @@
       <c r="K154" s="7" t="s">
         <v>1472</v>
       </c>
-      <c r="L154" s="8" t="s">
+      <c r="L154" s="13" t="s">
+        <v>1476</v>
+      </c>
+      <c r="M154" s="8" t="s">
         <v>1276</v>
       </c>
     </row>
-    <row r="155" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="155" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A155" t="s">
         <v>252</v>
       </c>
@@ -9619,8 +10103,11 @@
       <c r="K155" t="s">
         <v>1472</v>
       </c>
-    </row>
-    <row r="156" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="L155" s="13" t="s">
+        <v>1476</v>
+      </c>
+    </row>
+    <row r="156" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A156" t="s">
         <v>253</v>
       </c>
@@ -9648,8 +10135,11 @@
       <c r="K156" t="s">
         <v>1472</v>
       </c>
-    </row>
-    <row r="157" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="L156" s="13" t="s">
+        <v>1476</v>
+      </c>
+    </row>
+    <row r="157" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A157" t="s">
         <v>254</v>
       </c>
@@ -9677,8 +10167,11 @@
       <c r="K157" t="s">
         <v>1472</v>
       </c>
-    </row>
-    <row r="158" spans="1:12" s="13" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+      <c r="L157" s="13" t="s">
+        <v>1476</v>
+      </c>
+    </row>
+    <row r="158" spans="1:13" s="13" customFormat="1" ht="17" x14ac:dyDescent="0.2">
       <c r="A158" s="13" t="s">
         <v>255</v>
       </c>
@@ -9709,11 +10202,14 @@
       <c r="K158" s="13" t="s">
         <v>1472</v>
       </c>
-      <c r="L158" s="14" t="s">
+      <c r="L158" s="13" t="s">
+        <v>1476</v>
+      </c>
+      <c r="M158" s="14" t="s">
         <v>1278</v>
       </c>
     </row>
-    <row r="159" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="159" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A159" t="s">
         <v>256</v>
       </c>
@@ -9741,8 +10237,11 @@
       <c r="K159" t="s">
         <v>1472</v>
       </c>
-    </row>
-    <row r="160" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="L159" s="13" t="s">
+        <v>1476</v>
+      </c>
+    </row>
+    <row r="160" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A160" t="s">
         <v>257</v>
       </c>
@@ -9770,8 +10269,11 @@
       <c r="K160" t="s">
         <v>1472</v>
       </c>
-    </row>
-    <row r="161" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="L160" s="13" t="s">
+        <v>1476</v>
+      </c>
+    </row>
+    <row r="161" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A161" t="s">
         <v>258</v>
       </c>
@@ -9799,8 +10301,11 @@
       <c r="K161" t="s">
         <v>1472</v>
       </c>
-    </row>
-    <row r="162" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="L161" s="13" t="s">
+        <v>1476</v>
+      </c>
+    </row>
+    <row r="162" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A162" t="s">
         <v>259</v>
       </c>
@@ -9828,8 +10333,11 @@
       <c r="K162" t="s">
         <v>1472</v>
       </c>
-    </row>
-    <row r="163" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="L162" s="13" t="s">
+        <v>1476</v>
+      </c>
+    </row>
+    <row r="163" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A163" t="s">
         <v>260</v>
       </c>
@@ -9857,8 +10365,11 @@
       <c r="K163" t="s">
         <v>1472</v>
       </c>
-    </row>
-    <row r="164" spans="1:12" s="13" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+      <c r="L163" s="13" t="s">
+        <v>1476</v>
+      </c>
+    </row>
+    <row r="164" spans="1:13" s="13" customFormat="1" ht="17" x14ac:dyDescent="0.2">
       <c r="A164" s="13" t="s">
         <v>261</v>
       </c>
@@ -9889,11 +10400,14 @@
       <c r="K164" s="13" t="s">
         <v>1472</v>
       </c>
-      <c r="L164" s="14" t="s">
+      <c r="L164" s="13" t="s">
+        <v>1476</v>
+      </c>
+      <c r="M164" s="14" t="s">
         <v>1278</v>
       </c>
     </row>
-    <row r="165" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="165" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A165" t="s">
         <v>262</v>
       </c>
@@ -9921,8 +10435,11 @@
       <c r="K165" t="s">
         <v>1472</v>
       </c>
-    </row>
-    <row r="166" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="L165" s="13" t="s">
+        <v>1476</v>
+      </c>
+    </row>
+    <row r="166" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A166" t="s">
         <v>263</v>
       </c>
@@ -9950,8 +10467,11 @@
       <c r="K166" t="s">
         <v>1472</v>
       </c>
-    </row>
-    <row r="167" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="L166" s="13" t="s">
+        <v>1476</v>
+      </c>
+    </row>
+    <row r="167" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A167" t="s">
         <v>264</v>
       </c>
@@ -9979,8 +10499,11 @@
       <c r="K167" t="s">
         <v>1472</v>
       </c>
-    </row>
-    <row r="168" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="L167" s="13" t="s">
+        <v>1476</v>
+      </c>
+    </row>
+    <row r="168" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A168" t="s">
         <v>265</v>
       </c>
@@ -10008,8 +10531,11 @@
       <c r="K168" t="s">
         <v>1472</v>
       </c>
-    </row>
-    <row r="169" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="L168" s="13" t="s">
+        <v>1476</v>
+      </c>
+    </row>
+    <row r="169" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A169" t="s">
         <v>266</v>
       </c>
@@ -10037,8 +10563,11 @@
       <c r="K169" t="s">
         <v>1472</v>
       </c>
-    </row>
-    <row r="170" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="L169" s="13" t="s">
+        <v>1476</v>
+      </c>
+    </row>
+    <row r="170" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A170" t="s">
         <v>267</v>
       </c>
@@ -10066,8 +10595,11 @@
       <c r="K170" t="s">
         <v>1472</v>
       </c>
-    </row>
-    <row r="171" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="L170" s="13" t="s">
+        <v>1476</v>
+      </c>
+    </row>
+    <row r="171" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A171" t="s">
         <v>268</v>
       </c>
@@ -10095,8 +10627,11 @@
       <c r="K171" t="s">
         <v>1472</v>
       </c>
-    </row>
-    <row r="172" spans="1:12" s="13" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+      <c r="L171" s="13" t="s">
+        <v>1476</v>
+      </c>
+    </row>
+    <row r="172" spans="1:13" s="13" customFormat="1" ht="17" x14ac:dyDescent="0.2">
       <c r="A172" s="13" t="s">
         <v>269</v>
       </c>
@@ -10127,11 +10662,14 @@
       <c r="K172" s="13" t="s">
         <v>1472</v>
       </c>
-      <c r="L172" s="14" t="s">
+      <c r="L172" s="13" t="s">
+        <v>1476</v>
+      </c>
+      <c r="M172" s="14" t="s">
         <v>1278</v>
       </c>
     </row>
-    <row r="173" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="173" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A173" t="s">
         <v>270</v>
       </c>
@@ -10159,8 +10697,11 @@
       <c r="K173" t="s">
         <v>1472</v>
       </c>
-    </row>
-    <row r="174" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="L173" s="13" t="s">
+        <v>1476</v>
+      </c>
+    </row>
+    <row r="174" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A174" t="s">
         <v>271</v>
       </c>
@@ -10188,8 +10729,11 @@
       <c r="K174" t="s">
         <v>1472</v>
       </c>
-    </row>
-    <row r="175" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="L174" s="13" t="s">
+        <v>1476</v>
+      </c>
+    </row>
+    <row r="175" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A175" t="s">
         <v>272</v>
       </c>
@@ -10217,8 +10761,11 @@
       <c r="K175" t="s">
         <v>1472</v>
       </c>
-    </row>
-    <row r="176" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="L175" s="13" t="s">
+        <v>1476</v>
+      </c>
+    </row>
+    <row r="176" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A176" t="s">
         <v>273</v>
       </c>
@@ -10246,8 +10793,11 @@
       <c r="K176" t="s">
         <v>1472</v>
       </c>
-    </row>
-    <row r="177" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="L176" s="13" t="s">
+        <v>1476</v>
+      </c>
+    </row>
+    <row r="177" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A177" t="s">
         <v>274</v>
       </c>
@@ -10275,8 +10825,11 @@
       <c r="K177" t="s">
         <v>1472</v>
       </c>
-    </row>
-    <row r="178" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="L177" s="13" t="s">
+        <v>1476</v>
+      </c>
+    </row>
+    <row r="178" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A178" t="s">
         <v>275</v>
       </c>
@@ -10304,8 +10857,11 @@
       <c r="K178" t="s">
         <v>1472</v>
       </c>
-    </row>
-    <row r="179" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="L178" s="13" t="s">
+        <v>1476</v>
+      </c>
+    </row>
+    <row r="179" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A179" t="s">
         <v>276</v>
       </c>
@@ -10333,8 +10889,11 @@
       <c r="K179" t="s">
         <v>1472</v>
       </c>
-    </row>
-    <row r="180" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="L179" s="13" t="s">
+        <v>1476</v>
+      </c>
+    </row>
+    <row r="180" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A180" t="s">
         <v>277</v>
       </c>
@@ -10362,8 +10921,11 @@
       <c r="K180" t="s">
         <v>1472</v>
       </c>
-    </row>
-    <row r="181" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="L180" s="13" t="s">
+        <v>1476</v>
+      </c>
+    </row>
+    <row r="181" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A181" t="s">
         <v>278</v>
       </c>
@@ -10391,8 +10953,11 @@
       <c r="K181" t="s">
         <v>1472</v>
       </c>
-    </row>
-    <row r="182" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="L181" s="13" t="s">
+        <v>1476</v>
+      </c>
+    </row>
+    <row r="182" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A182" t="s">
         <v>279</v>
       </c>
@@ -10420,8 +10985,11 @@
       <c r="K182" t="s">
         <v>1472</v>
       </c>
-    </row>
-    <row r="183" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="L182" s="13" t="s">
+        <v>1476</v>
+      </c>
+    </row>
+    <row r="183" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A183" t="s">
         <v>280</v>
       </c>
@@ -10449,8 +11017,11 @@
       <c r="K183" t="s">
         <v>1472</v>
       </c>
-    </row>
-    <row r="184" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="L183" s="13" t="s">
+        <v>1476</v>
+      </c>
+    </row>
+    <row r="184" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A184" t="s">
         <v>281</v>
       </c>
@@ -10478,8 +11049,11 @@
       <c r="K184" t="s">
         <v>1472</v>
       </c>
-    </row>
-    <row r="185" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="L184" s="13" t="s">
+        <v>1476</v>
+      </c>
+    </row>
+    <row r="185" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A185" t="s">
         <v>282</v>
       </c>
@@ -10507,8 +11081,11 @@
       <c r="K185" t="s">
         <v>1472</v>
       </c>
-    </row>
-    <row r="186" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="L185" s="13" t="s">
+        <v>1476</v>
+      </c>
+    </row>
+    <row r="186" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A186" t="s">
         <v>283</v>
       </c>
@@ -10536,8 +11113,11 @@
       <c r="K186" t="s">
         <v>1472</v>
       </c>
-    </row>
-    <row r="187" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="L186" s="13" t="s">
+        <v>1476</v>
+      </c>
+    </row>
+    <row r="187" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A187" t="s">
         <v>284</v>
       </c>
@@ -10565,9 +11145,12 @@
       <c r="K187" t="s">
         <v>1466</v>
       </c>
-      <c r="L187"/>
-    </row>
-    <row r="188" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="L187" s="13" t="s">
+        <v>1476</v>
+      </c>
+      <c r="M187"/>
+    </row>
+    <row r="188" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A188" t="s">
         <v>285</v>
       </c>
@@ -10595,9 +11178,12 @@
       <c r="K188" t="s">
         <v>1466</v>
       </c>
-      <c r="L188"/>
-    </row>
-    <row r="189" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="L188" s="13" t="s">
+        <v>1476</v>
+      </c>
+      <c r="M188"/>
+    </row>
+    <row r="189" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A189" t="s">
         <v>286</v>
       </c>
@@ -10625,9 +11211,12 @@
       <c r="K189" t="s">
         <v>1466</v>
       </c>
-      <c r="L189"/>
-    </row>
-    <row r="190" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="L189" s="13" t="s">
+        <v>1476</v>
+      </c>
+      <c r="M189"/>
+    </row>
+    <row r="190" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A190" t="s">
         <v>287</v>
       </c>
@@ -10655,9 +11244,12 @@
       <c r="K190" t="s">
         <v>1466</v>
       </c>
-      <c r="L190"/>
-    </row>
-    <row r="191" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="L190" t="s">
+        <v>1477</v>
+      </c>
+      <c r="M190"/>
+    </row>
+    <row r="191" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A191" t="s">
         <v>288</v>
       </c>
@@ -10685,9 +11277,12 @@
       <c r="K191" t="s">
         <v>1466</v>
       </c>
-      <c r="L191"/>
-    </row>
-    <row r="192" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="L191" s="13" t="s">
+        <v>1476</v>
+      </c>
+      <c r="M191"/>
+    </row>
+    <row r="192" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A192" t="s">
         <v>289</v>
       </c>
@@ -10715,9 +11310,12 @@
       <c r="K192" t="s">
         <v>1466</v>
       </c>
-      <c r="L192"/>
-    </row>
-    <row r="193" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="L192" s="13" t="s">
+        <v>1476</v>
+      </c>
+      <c r="M192"/>
+    </row>
+    <row r="193" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A193" t="s">
         <v>290</v>
       </c>
@@ -10745,9 +11343,12 @@
       <c r="K193" t="s">
         <v>1466</v>
       </c>
-      <c r="L193"/>
-    </row>
-    <row r="194" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="L193" s="13" t="s">
+        <v>1476</v>
+      </c>
+      <c r="M193"/>
+    </row>
+    <row r="194" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A194" t="s">
         <v>291</v>
       </c>
@@ -10775,9 +11376,12 @@
       <c r="K194" t="s">
         <v>1466</v>
       </c>
-      <c r="L194"/>
-    </row>
-    <row r="195" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="L194" t="s">
+        <v>1477</v>
+      </c>
+      <c r="M194"/>
+    </row>
+    <row r="195" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A195" t="s">
         <v>292</v>
       </c>
@@ -10805,9 +11409,12 @@
       <c r="K195" t="s">
         <v>1466</v>
       </c>
-      <c r="L195"/>
-    </row>
-    <row r="196" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="L195" t="s">
+        <v>1477</v>
+      </c>
+      <c r="M195"/>
+    </row>
+    <row r="196" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A196" t="s">
         <v>293</v>
       </c>
@@ -10835,9 +11442,12 @@
       <c r="K196" t="s">
         <v>1466</v>
       </c>
-      <c r="L196"/>
-    </row>
-    <row r="197" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="L196" t="s">
+        <v>1477</v>
+      </c>
+      <c r="M196"/>
+    </row>
+    <row r="197" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A197" t="s">
         <v>294</v>
       </c>
@@ -10859,11 +11469,11 @@
       <c r="K197" t="s">
         <v>1467</v>
       </c>
-      <c r="L197" t="s">
+      <c r="M197" t="s">
         <v>528</v>
       </c>
     </row>
-    <row r="198" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="198" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A198" t="s">
         <v>295</v>
       </c>
@@ -10893,9 +11503,12 @@
       <c r="K198" t="s">
         <v>1469</v>
       </c>
-      <c r="L198"/>
-    </row>
-    <row r="199" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="L198" t="s">
+        <v>1478</v>
+      </c>
+      <c r="M198"/>
+    </row>
+    <row r="199" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A199" t="s">
         <v>296</v>
       </c>
@@ -10925,9 +11538,12 @@
       <c r="K199" t="s">
         <v>1469</v>
       </c>
-      <c r="L199"/>
-    </row>
-    <row r="200" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="L199" t="s">
+        <v>1478</v>
+      </c>
+      <c r="M199"/>
+    </row>
+    <row r="200" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A200" t="s">
         <v>297</v>
       </c>
@@ -10957,9 +11573,12 @@
       <c r="K200" t="s">
         <v>1468</v>
       </c>
-      <c r="L200"/>
-    </row>
-    <row r="201" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="L200" t="s">
+        <v>1478</v>
+      </c>
+      <c r="M200"/>
+    </row>
+    <row r="201" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A201" t="s">
         <v>298</v>
       </c>
@@ -10989,8 +11608,11 @@
       <c r="K201" t="s">
         <v>1470</v>
       </c>
-    </row>
-    <row r="202" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="L201" t="s">
+        <v>1477</v>
+      </c>
+    </row>
+    <row r="202" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A202" t="s">
         <v>299</v>
       </c>
@@ -11020,8 +11642,11 @@
       <c r="K202" t="s">
         <v>1470</v>
       </c>
-    </row>
-    <row r="203" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="L202" t="s">
+        <v>1477</v>
+      </c>
+    </row>
+    <row r="203" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A203" t="s">
         <v>300</v>
       </c>
@@ -11049,8 +11674,11 @@
       <c r="K203" t="s">
         <v>1471</v>
       </c>
-    </row>
-    <row r="204" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="L203" t="s">
+        <v>1477</v>
+      </c>
+    </row>
+    <row r="204" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A204" t="s">
         <v>301</v>
       </c>
@@ -11078,8 +11706,11 @@
       <c r="K204" t="s">
         <v>1471</v>
       </c>
-    </row>
-    <row r="205" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="L204" t="s">
+        <v>1477</v>
+      </c>
+    </row>
+    <row r="205" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A205" t="s">
         <v>302</v>
       </c>
@@ -11107,8 +11738,12 @@
       <c r="K205" t="s">
         <v>1471</v>
       </c>
+      <c r="L205" t="s">
+        <v>1477</v>
+      </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>